<commit_message>
ToDo, CodeConventions, sql script, logo
ToDo geupdate, CodeConvetions toegevoegd, gh4_sqlserver.sql script
toegevoegd, logo toegevoegd
</commit_message>
<xml_diff>
--- a/ToDo_Deel2.xlsx
+++ b/ToDo_Deel2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Code conventions opstellen</t>
+  </si>
+  <si>
+    <t>15 min</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-BE"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -487,7 +490,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,7 +519,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -877,7 +880,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1039,7 @@
       </c>
       <c r="J7" s="13">
         <f>I7/$I$10</f>
-        <v>0.42857142857142855</v>
+        <v>0.375</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>12</v>
@@ -1074,11 +1077,11 @@
       <c r="H9" s="2"/>
       <c r="I9" s="17">
         <f>COUNTIFS(A2:G2038,"Solved")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J9" s="18">
         <f>I9/$I$10</f>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>4</v>
@@ -1095,7 +1098,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="20">
         <f>SUM(I6:I9)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J10" s="21">
         <v>1</v>
@@ -1238,15 +1241,24 @@
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="23">
+        <v>41762</v>
+      </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>

</xml_diff>